<commit_message>
+Worked on sending mail process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Day10_Assignment2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day_10a\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADFB7DA-6A7C-4A5B-B45B-7BBF5035EC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EAFA5A-8EAB-4CB2-83E1-FEBD11CCA7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>257175</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -298,7 +298,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBEB2A4F-A08B-E130-E310-6E64FD296E5C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -708,7 +708,14 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2875,8 +2882,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2935,12 +2942,6 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
@@ -3965,7 +3966,7 @@
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>

</xml_diff>